<commit_message>
improved Threading with QRunnables, improved and added firewall service functions incl. testing
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -179,6 +179,9 @@
     <t xml:space="preserve">rekursiv, Ordnerbasiert, funktioniert, Testautomation und GUI ok; erfordert Ablageordner auf clientseitig erreichbarem CIFS-Share</t>
   </si>
   <si>
+    <t xml:space="preserve">TODO: prüfe Client-Namen</t>
+  </si>
+  <si>
     <t xml:space="preserve">clientseitige Prüfungsdateien in App monitoren</t>
   </si>
   <si>
@@ -209,7 +212,7 @@
     <t xml:space="preserve">clientseitige Firewall-Configuration</t>
   </si>
   <si>
-    <t xml:space="preserve">parameterisierbare Funktion zum Erstellen und Löschen von Firewall-Regeln exisitiert; inkl.UnitTest; LB-Kandidaten dürfen max "Hauptbenutzer" sein</t>
+    <t xml:space="preserve">parameterisierbare Funktion zum Erstellen und Löschen von Firewall-Regeln exisitiert; inkl.UnitTest; LB-Kandidaten dürfen max "Hauptbenutzer" sein; Stolperstein: globaler Firewall-Service Zustand gelöst</t>
   </si>
   <si>
     <t xml:space="preserve">USB-Ports deaktivieren</t>
@@ -251,7 +254,7 @@
     <t xml:space="preserve">Modale Progressbars?</t>
   </si>
   <si>
-    <t xml:space="preserve">sauberes Threading mit QThreads und Workers implementiert, ProgressBar am unteren Bildschirmrand funktioniert ordentlich</t>
+    <t xml:space="preserve">sauberes Threading mit QThreads und Workers (QRunnables in ThreadPools) implementiert, ProgressBar am unteren Bildschirmrand funktioniert ordentlich</t>
   </si>
   <si>
     <t xml:space="preserve">Config-File und Konfigurationsdialog</t>
@@ -770,8 +773,8 @@
   </sheetPr>
   <dimension ref="A1:G30"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D30" activeCellId="0" sqref="D30"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -917,11 +920,13 @@
       <c r="E7" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="1"/>
+      <c r="F7" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="10" t="n">
         <v>4</v>
@@ -933,13 +938,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="B9" s="10" t="n">
         <v>4</v>
@@ -951,12 +956,12 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="10" t="n">
         <v>4</v>
@@ -968,66 +973,66 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="B11" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C11" s="12" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D11" s="10" t="n">
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>8</v>
       </c>
       <c r="C13" s="12" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D13" s="10" t="n">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="B14" s="10" t="n">
         <v>4</v>
       </c>
       <c r="C14" s="12" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>8</v>
@@ -1036,12 +1041,12 @@
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" s="18" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B19" s="16" t="n">
         <f aca="false">SUM(B2:B18)</f>
@@ -1049,18 +1054,18 @@
       </c>
       <c r="C19" s="17" t="n">
         <f aca="false">AVERAGE(C2:C18)</f>
-        <v>0.8</v>
+        <v>0.825</v>
       </c>
       <c r="D19" s="16" t="n">
         <f aca="false">SUM(D2:D18)</f>
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1070,7 +1075,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>8</v>
@@ -1082,12 +1087,12 @@
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>8</v>
@@ -1099,12 +1104,12 @@
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="26" s="6" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -1114,7 +1119,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0.5</v>
@@ -1126,26 +1131,26 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>2</v>
       </c>
       <c r="C28" s="12" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>4</v>
@@ -1159,7 +1164,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added remote status handling and reset functionality
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -206,7 +206,7 @@
     <t xml:space="preserve">create Windows-Installation für LB-Deploy-GUI</t>
   </si>
   <si>
-    <t xml:space="preserve">works with pyinstaller</t>
+    <t xml:space="preserve">funktioniert für Windows 10 mit pyinstaller</t>
   </si>
   <si>
     <t xml:space="preserve">clientseitige Firewall-Configuration</t>
@@ -218,7 +218,7 @@
     <t xml:space="preserve">USB-Ports deaktivieren</t>
   </si>
   <si>
-    <t xml:space="preserve">works for computer class and LbClient Button</t>
+    <t xml:space="preserve">done</t>
   </si>
   <si>
     <t xml:space="preserve">Projektmanagement (Angebote, KOmmunikation, Excel)</t>
@@ -260,7 +260,57 @@
     <t xml:space="preserve">Config-File und Konfigurationsdialog</t>
   </si>
   <si>
-    <t xml:space="preserve">Bugfixes Testing</t>
+    <t xml:space="preserve">Bugfixes Testing (again and again)</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">IMPORTANT MISSING FEATURE: maintain state file on </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">clientside </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">including </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">reset</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> to allow restart of app / rescan of clients</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Hilfe-File</t>
   </si>
 </sst>
 </file>
@@ -271,7 +321,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -306,6 +356,11 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -771,10 +826,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G30"/>
+  <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1166,9 +1221,37 @@
       <c r="A30" s="2" t="s">
         <v>67</v>
       </c>
+      <c r="D30" s="10" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="10" t="n">
+        <v>8</v>
+      </c>
+      <c r="C31" s="12" t="n">
+        <v>0.85</v>
+      </c>
+      <c r="D31" s="10" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C32" s="10" t="n">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C29">
+  <conditionalFormatting sqref="C2:C50">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="num" val="0"/>

</xml_diff>

<commit_message>
added bulk candidate name feature (using a new UI tab); discovered a flaw in the bulk reset (still unsolved)
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -128,7 +128,25 @@
     <t xml:space="preserve">Kandidatennamen für Client verwalten</t>
   </si>
   <si>
-    <t xml:space="preserve">Kandidatenname kann von App zugewiesen und ausgelesen werden, Möglichkeit zur clientseitigen Eingabe des Kandidaten-Namen besteht</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Kandidatenname kann von App zugewiesen und ausgelesen werden, Möglichkeit zur clientseitigen Eingabe des Kandidaten-Namen besteht; </t>
+    </r>
+    <r>
+      <rPr>
+        <b val="true"/>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Usability: Kandidatennamen per Liste batchzuweisen geht</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Kandidatennamen auf Eindeutigkeit prüfen; mit SOLL-Liste abgleichen oder von SOLL-Liste zuweisen?</t>
@@ -270,24 +288,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">IMPORTANT MISSING FEATURE: maintain state file on </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">clientside </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">including </t>
+      <t xml:space="preserve">IMPORTANT MISSING FEATURE: maintain state file on clientside including </t>
     </r>
     <r>
       <rPr>
@@ -310,6 +311,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve"> TODO FIXME: programmabsturz, wenn Kandidatennamen ebenfalls zurückgesetzt werden!</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hilfe-File</t>
   </si>
 </sst>
@@ -321,7 +325,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="0.00%"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -356,11 +360,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -829,7 +828,7 @@
   <dimension ref="A1:G32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C32" activeCellId="0" sqref="C32"/>
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -896,7 +895,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
         <v>28</v>
       </c>
@@ -904,10 +903,10 @@
         <v>8</v>
       </c>
       <c r="C4" s="12" t="n">
-        <v>0.8</v>
+        <v>0.9</v>
       </c>
       <c r="D4" s="10" t="n">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>29</v>
@@ -1109,11 +1108,11 @@
       </c>
       <c r="C19" s="17" t="n">
         <f aca="false">AVERAGE(C2:C18)</f>
-        <v>0.825</v>
+        <v>0.833333333333333</v>
       </c>
       <c r="D19" s="16" t="n">
         <f aca="false">SUM(D2:D18)</f>
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1238,10 +1237,13 @@
       <c r="D31" s="10" t="n">
         <v>8</v>
       </c>
+      <c r="E31" s="13" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="10" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
still trying to fix bugs for reset and proper copy process for shares
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -182,6 +182,9 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">Wichtig: Benutzer-Account auf Client muss vollständig erstellt sein, bevor das erste mal kopiert wird. Standardbenutzer student vereinfacht alles!; TODO: Test Datei- und Netzwerkfreigabe für aktuelle Netzwerkverbindung auf WISS-Image</t>
+  </si>
+  <si>
     <t xml:space="preserve">Win-Deployment PC: automatisch share für ausgewählte LB-Verzeichnisse generieren</t>
   </si>
   <si>
@@ -279,6 +282,9 @@
   </si>
   <si>
     <t xml:space="preserve">Bugfixes Testing (again and again)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bugs fixed: Crash on reset all clients (switch from stylesheet to direct button format)</t>
   </si>
   <si>
     <r>
@@ -827,8 +833,8 @@
   </sheetPr>
   <dimension ref="A1:G32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -937,10 +943,13 @@
       <c r="F5" s="1" t="s">
         <v>34</v>
       </c>
+      <c r="G5" s="6" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="13" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>3</v>
@@ -952,15 +961,15 @@
         <v>6</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>6</v>
@@ -972,15 +981,15 @@
         <v>9</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="13" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B8" s="10" t="n">
         <v>4</v>
@@ -992,13 +1001,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="F8" s="0"/>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B9" s="10" t="n">
         <v>4</v>
@@ -1010,12 +1019,12 @@
         <v>4</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="B10" s="10" t="n">
         <v>4</v>
@@ -1027,15 +1036,15 @@
         <v>3</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="B11" s="10" t="n">
         <v>2</v>
@@ -1047,12 +1056,12 @@
         <v>4</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>8</v>
@@ -1064,12 +1073,12 @@
         <v>8</v>
       </c>
       <c r="E13" s="14" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B14" s="10" t="n">
         <v>4</v>
@@ -1081,12 +1090,12 @@
         <v>2</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>8</v>
@@ -1095,12 +1104,12 @@
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="19" s="18" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="15" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B19" s="16" t="n">
         <f aca="false">SUM(B2:B18)</f>
@@ -1119,7 +1128,7 @@
     </row>
     <row r="21" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1129,7 +1138,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>8</v>
@@ -1141,12 +1150,12 @@
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>8</v>
@@ -1158,12 +1167,12 @@
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
     <row r="26" s="6" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="B26" s="19"/>
       <c r="C26" s="19"/>
@@ -1173,7 +1182,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0.5</v>
@@ -1187,7 +1196,7 @@
     </row>
     <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>2</v>
@@ -1199,12 +1208,12 @@
         <v>7</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>4</v>
@@ -1216,17 +1225,20 @@
         <v>4</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="D30" s="10" t="n">
-        <v>6</v>
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>8</v>
@@ -1238,12 +1250,12 @@
         <v>8</v>
       </c>
       <c r="E31" s="13" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B32" s="10" t="n">
         <v>4</v>

</xml_diff>

<commit_message>
added sharebrowser module as preparation for wizard based exam selection; basic tests (in main) work on UNIX and WIN clients as well as for UNIX und WIN shares
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">rekursiv, Ordnerbasiert, funktioniert, Testautomation und GUI ok; erfordert Ablageordner auf clientseitig erreichbarem CIFS-Share</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO: prüfe Client-Namen</t>
+    <t xml:space="preserve">TODO: prüfe Client-Namen; übergebe User/Password von App an Subsysteme --&gt; smbbrowser-modul</t>
   </si>
   <si>
     <t xml:space="preserve">clientseitige Prüfungsdateien in App monitoren</t>
@@ -321,6 +321,9 @@
   </si>
   <si>
     <t xml:space="preserve">Hilfe-File</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wizard für user/password basierte Modulauswahl</t>
   </si>
 </sst>
 </file>
@@ -831,10 +834,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G32"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G5" activeCellId="0" sqref="G5"/>
+      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -967,7 +970,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
@@ -978,7 +981,7 @@
         <v>0.8</v>
       </c>
       <c r="D7" s="10" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>40</v>
@@ -1121,7 +1124,7 @@
       </c>
       <c r="D19" s="16" t="n">
         <f aca="false">SUM(D2:D18)</f>
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="E19" s="15"/>
       <c r="F19" s="15"/>
@@ -1262,6 +1265,20 @@
       </c>
       <c r="C32" s="10" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B33" s="10" t="n">
+        <v>16</v>
+      </c>
+      <c r="C33" s="12" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D33" s="10" t="n">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
reworked most GUI threads using ProgressDialog; added preliminary Candidate2LockScreen feature; reworked reset --> now whipes entire Desktop;
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -324,6 +324,27 @@
   </si>
   <si>
     <t xml:space="preserve">Wizard für user/password basierte Modulauswahl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rework Progress (einmal mehr, nach Abstürzen beim Multi-Client Test)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.03.19: ECMan crasht bzw. Progressbars nicht funktional bei Tests mit 12+ Clients; insbesondere RESET, SetCandidatename betroffen (fehlerhaftes Handling der notifications)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISSUES:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hauptbenutzer können Firewall deaktivieren:  Windows10-Version 2016LTSB)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">offen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CIFS Shares</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fixed</t>
   </si>
 </sst>
 </file>
@@ -371,7 +392,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -382,6 +403,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFDDDDDD"/>
         <bgColor rgb="FFCCFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFF200"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00CC00"/>
+        <bgColor rgb="FF008000"/>
       </patternFill>
     </fill>
   </fills>
@@ -419,7 +452,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -497,6 +530,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,9 +555,9 @@
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
       <rgbColor rgb="FFFF0000"/>
-      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF00CC00"/>
       <rgbColor rgb="FF0000FF"/>
-      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFFF200"/>
       <rgbColor rgb="FFFF00FF"/>
       <rgbColor rgb="FF00FFFF"/>
       <rgbColor rgb="FF800000"/>
@@ -834,10 +875,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G33"/>
+  <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C7" activeCellId="0" sqref="C7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1275,15 +1316,57 @@
         <v>16</v>
       </c>
       <c r="C33" s="12" t="n">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="D33" s="10" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" s="10" t="n">
         <v>4</v>
       </c>
+      <c r="E34" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B37" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="C37" s="20" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B38" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="C38" s="21" t="s">
+        <v>80</v>
+      </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C2:C50">
+  <conditionalFormatting sqref="C39:C50 C2:C36">
     <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="num" val="0"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="num" val="1"/>
+        <color rgb="FFFF0000"/>
+        <color rgb="FFFFFF00"/>
+        <color rgb="FF00CC00"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C38">
+    <cfRule type="colorScale" priority="3">
       <colorScale>
         <cfvo type="num" val="0"/>
         <cfvo type="percentile" val="50"/>

</xml_diff>

<commit_message>
improved candidate name display in lock screen; started PDF export for individual client logs
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -215,7 +215,7 @@
     <t xml:space="preserve">ConfigureRemotingForAnsible.ps1</t>
   </si>
   <si>
-    <t xml:space="preserve">Fehlerprotokollierung</t>
+    <t xml:space="preserve">LB-Deployment: Ablauf-Protokollierung</t>
   </si>
   <si>
     <t xml:space="preserve">innerhalb LbClient sammeln, in GUI HTML-formatiert ausgeben</t>
@@ -242,6 +242,9 @@
     <t xml:space="preserve">done</t>
   </si>
   <si>
+    <t xml:space="preserve">Hilfe-File</t>
+  </si>
+  <si>
     <t xml:space="preserve">Projektmanagement (Angebote, KOmmunikation, Excel)</t>
   </si>
   <si>
@@ -276,6 +279,9 @@
   </si>
   <si>
     <t xml:space="preserve">sauberes Threading mit QThreads und Workers (QRunnables in ThreadPools) implementiert, ProgressBar am unteren Bildschirmrand funktioniert ordentlich</t>
+  </si>
+  <si>
+    <t xml:space="preserve">04.03.19: ECMan crasht bzw. Progressbars nicht funktional bei Tests mit 12+ Clients; insbesondere RESET, SetCandidatename betroffen (fehlerhaftes Handling der notifications)</t>
   </si>
   <si>
     <t xml:space="preserve">Config-File und Konfigurationsdialog</t>
@@ -317,19 +323,13 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve"> TODO FIXME: programmabsturz, wenn Kandidatennamen ebenfalls zurückgesetzt werden!</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hilfe-File</t>
-  </si>
-  <si>
     <t xml:space="preserve">Wizard für user/password basierte Modulauswahl</t>
   </si>
   <si>
-    <t xml:space="preserve">Rework Progress (einmal mehr, nach Abstürzen beim Multi-Client Test)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">04.03.19: ECMan crasht bzw. Progressbars nicht funktional bei Tests mit 12+ Clients; insbesondere RESET, SetCandidatename betroffen (fehlerhaftes Handling der notifications)</t>
+    <t xml:space="preserve">Kandidatennamen im Login Screen anzeigen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">wichtige Änderung: Configure4Ansible installiert imagemagick und passt Berechtigungen zum Verändern des Lock-Bildes an; TODO: GPO muss angepasst werden (und das CMDLET tut nicht...</t>
   </si>
   <si>
     <t xml:space="preserve">ISSUES:</t>
@@ -342,9 +342,6 @@
   </si>
   <si>
     <t xml:space="preserve">CIFS Shares</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fixed</t>
   </si>
 </sst>
 </file>
@@ -498,10 +495,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -529,15 +530,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -550,6 +547,16 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="2">
+    <dxf/>
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+      </font>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -877,21 +884,23 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="2" width="43.78"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="2" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="2" min="2" style="10" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="3" min="3" style="11" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="4" min="4" style="10" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="60.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="31.28"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="7" style="0" width="11.52"/>
   </cols>
   <sheetData>
-    <row r="1" s="11" customFormat="true" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="11" t="s">
+    <row r="1" s="12" customFormat="true" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B1" s="7" t="s">
@@ -906,7 +915,7 @@
       <c r="E1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="F1" s="12" t="s">
         <v>23</v>
       </c>
     </row>
@@ -917,13 +926,13 @@
       <c r="B2" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C2" s="12" t="n">
-        <v>0.8</v>
+      <c r="C2" s="13" t="n">
+        <v>0.9</v>
       </c>
       <c r="D2" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E2" s="0" t="s">
+      <c r="E2" s="14" t="s">
         <v>25</v>
       </c>
       <c r="F2" s="0"/>
@@ -935,7 +944,7 @@
       <c r="B3" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C3" s="12" t="n">
+      <c r="C3" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D3" s="10" t="n">
@@ -952,7 +961,7 @@
       <c r="B4" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C4" s="12" t="n">
+      <c r="C4" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D4" s="10" t="n">
@@ -975,8 +984,8 @@
       <c r="B5" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C5" s="12" t="n">
-        <v>0.8</v>
+      <c r="C5" s="13" t="n">
+        <v>0.9</v>
       </c>
       <c r="D5" s="10" t="n">
         <v>8</v>
@@ -991,14 +1000,14 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="13" t="s">
+    <row r="6" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="10" t="n">
         <v>3</v>
       </c>
-      <c r="C6" s="12" t="n">
+      <c r="C6" s="13" t="n">
         <v>0.7</v>
       </c>
       <c r="D6" s="10" t="n">
@@ -1011,15 +1020,15 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="B7" s="10" t="n">
         <v>6</v>
       </c>
-      <c r="C7" s="12" t="n">
-        <v>0.8</v>
+      <c r="C7" s="13" t="n">
+        <v>0.9</v>
       </c>
       <c r="D7" s="10" t="n">
         <v>12</v>
@@ -1032,13 +1041,13 @@
       </c>
     </row>
     <row r="8" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="14" t="s">
         <v>42</v>
       </c>
       <c r="B8" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C8" s="12" t="n">
+      <c r="C8" s="13" t="n">
         <v>0.8</v>
       </c>
       <c r="D8" s="10" t="n">
@@ -1056,8 +1065,8 @@
       <c r="B9" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C9" s="12" t="n">
-        <v>0.8</v>
+      <c r="C9" s="13" t="n">
+        <v>0.9</v>
       </c>
       <c r="D9" s="10" t="n">
         <v>4</v>
@@ -1066,15 +1075,15 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
       <c r="B10" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C10" s="12" t="n">
-        <v>0.8</v>
+      <c r="C10" s="13" t="n">
+        <v>0.4</v>
       </c>
       <c r="D10" s="10" t="n">
         <v>3</v>
@@ -1093,7 +1102,7 @@
       <c r="B11" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C11" s="12" t="n">
+      <c r="C11" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D11" s="10" t="n">
@@ -1103,20 +1112,20 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="s">
         <v>51</v>
       </c>
       <c r="B13" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C13" s="12" t="n">
+      <c r="C13" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D13" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="E13" s="14" t="s">
+      <c r="E13" s="15" t="s">
         <v>52</v>
       </c>
     </row>
@@ -1127,19 +1136,30 @@
       <c r="B14" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C14" s="12" t="n">
+      <c r="C14" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D14" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="E14" s="0" t="s">
+      <c r="E14" s="14" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="24.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B15" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C15" s="13" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B17" s="10" t="n">
         <v>8</v>
@@ -1148,165 +1168,160 @@
         <v>8</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="19" s="18" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="15" t="s">
         <v>57</v>
       </c>
-      <c r="B19" s="16" t="n">
+    </row>
+    <row r="19" s="19" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="B19" s="17" t="n">
         <f aca="false">SUM(B2:B18)</f>
-        <v>71</v>
-      </c>
-      <c r="C19" s="17" t="n">
+        <v>75</v>
+      </c>
+      <c r="C19" s="18" t="n">
         <f aca="false">AVERAGE(C2:C18)</f>
-        <v>0.833333333333333</v>
-      </c>
-      <c r="D19" s="16" t="n">
+        <v>0.769230769230769</v>
+      </c>
+      <c r="D19" s="17" t="n">
         <f aca="false">SUM(D2:D18)</f>
         <v>87</v>
       </c>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
     </row>
     <row r="21" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B21" s="19"/>
-      <c r="C21" s="19"/>
-      <c r="D21" s="19"/>
+        <v>59</v>
+      </c>
+      <c r="B21" s="11"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="11"/>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
-    <row r="22" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B22" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C22" s="12" t="n">
+      <c r="C22" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="D22" s="10" t="n">
         <v>2</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="2" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B23" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C23" s="12" t="n">
+      <c r="C23" s="13" t="n">
         <v>0.1</v>
       </c>
       <c r="D23" s="10" t="n">
         <v>1</v>
       </c>
       <c r="E23" s="2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="26" s="6" customFormat="true" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" s="6" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="B26" s="19"/>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
+        <v>64</v>
+      </c>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11"/>
       <c r="E26" s="1"/>
       <c r="F26" s="1"/>
     </row>
-    <row r="27" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B27" s="10" t="n">
         <v>0.5</v>
       </c>
-      <c r="C27" s="12" t="n">
+      <c r="C27" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D27" s="10" t="n">
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B28" s="10" t="n">
         <v>2</v>
       </c>
-      <c r="C28" s="12" t="n">
+      <c r="C28" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>7</v>
+        <v>11</v>
       </c>
       <c r="E28" s="2" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>67</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="2" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B29" s="10" t="n">
         <v>4</v>
       </c>
-      <c r="C29" s="12" t="n">
+      <c r="C29" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D29" s="10" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="2" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D30" s="10" t="n">
         <v>8</v>
       </c>
       <c r="E30" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B31" s="10" t="n">
         <v>8</v>
       </c>
-      <c r="C31" s="12" t="n">
-        <v>0.85</v>
+      <c r="C31" s="13" t="n">
+        <v>0.9</v>
       </c>
       <c r="D31" s="10" t="n">
-        <v>8</v>
-      </c>
-      <c r="E31" s="13" t="s">
-        <v>71</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="E31" s="14"/>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B32" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="C32" s="10" t="n">
-        <v>0</v>
-      </c>
+      <c r="A32" s="0"/>
+      <c r="B32" s="0"/>
+      <c r="C32" s="6"/>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
@@ -1315,7 +1330,7 @@
       <c r="B33" s="10" t="n">
         <v>16</v>
       </c>
-      <c r="C33" s="12" t="n">
+      <c r="C33" s="13" t="n">
         <v>0.9</v>
       </c>
       <c r="D33" s="10" t="n">
@@ -1326,10 +1341,16 @@
       <c r="A34" s="2" t="s">
         <v>74</v>
       </c>
+      <c r="B34" s="10" t="n">
+        <v>4</v>
+      </c>
+      <c r="C34" s="13" t="n">
+        <v>0.9</v>
+      </c>
       <c r="D34" s="10" t="n">
-        <v>4</v>
-      </c>
-      <c r="E34" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E34" s="14" t="s">
         <v>75</v>
       </c>
     </row>
@@ -1337,7 +1358,7 @@
       <c r="A37" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="15" t="s">
         <v>77</v>
       </c>
       <c r="C37" s="20" t="s">
@@ -1348,33 +1369,21 @@
       <c r="B38" s="10" t="s">
         <v>79</v>
       </c>
-      <c r="C38" s="21" t="s">
-        <v>80</v>
+      <c r="C38" s="21" t="n">
+        <v>0.9</v>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="C39:C50 C2:C36">
-    <cfRule type="colorScale" priority="2">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF00CC00"/>
-      </colorScale>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="cellIs" priority="2" operator="lessThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>50%</formula>
     </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C38">
-    <cfRule type="colorScale" priority="3">
-      <colorScale>
-        <cfvo type="num" val="0"/>
-        <cfvo type="percentile" val="50"/>
-        <cfvo type="num" val="1"/>
-        <color rgb="FFFF0000"/>
-        <color rgb="FFFFFF00"/>
-        <color rgb="FF00CC00"/>
-      </colorScale>
+    <cfRule type="cellIs" priority="3" operator="between" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>50%</formula>
+      <formula>80%</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="greaterThan" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>80%</formula>
     </cfRule>
   </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
added logfile printing functionality
</commit_message>
<xml_diff>
--- a/projektmanagement.xlsx
+++ b/projektmanagement.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="82">
   <si>
     <t xml:space="preserve">Internal Logical File</t>
   </si>
@@ -221,7 +221,8 @@
     <t xml:space="preserve">innerhalb LbClient sammeln, in GUI HTML-formatiert ausgeben</t>
   </si>
   <si>
-    <t xml:space="preserve">TODO: Protokolle als PDF im Ergebnisordner ablegen</t>
+    <t xml:space="preserve">TODO: Protokolle als PDF im Ergebnisordner ablegen;
+Protokolle auf ECMan-Dozentenpc auch mal löschen</t>
   </si>
   <si>
     <t xml:space="preserve">create Windows-Installation für LB-Deploy-GUI</t>
@@ -281,7 +282,7 @@
     <t xml:space="preserve">sauberes Threading mit QThreads und Workers (QRunnables in ThreadPools) implementiert, ProgressBar am unteren Bildschirmrand funktioniert ordentlich</t>
   </si>
   <si>
-    <t xml:space="preserve">04.03.19: ECMan crasht bzw. Progressbars nicht funktional bei Tests mit 12+ Clients; insbesondere RESET, SetCandidatename betroffen (fehlerhaftes Handling der notifications)</t>
+    <t xml:space="preserve">Probleme beim mehrfachen Scannen des netzwerks, LBClient-Widgets falsch entfernt</t>
   </si>
   <si>
     <t xml:space="preserve">Config-File und Konfigurationsdialog</t>
@@ -323,13 +324,19 @@
     </r>
   </si>
   <si>
+    <t xml:space="preserve">erledigt</t>
+  </si>
+  <si>
     <t xml:space="preserve">Wizard für user/password basierte Modulauswahl</t>
   </si>
   <si>
+    <t xml:space="preserve">viel Aufwand und Ärger mit verschiedenen SMB-Server Konfigurationen</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kandidatennamen im Login Screen anzeigen</t>
   </si>
   <si>
-    <t xml:space="preserve">wichtige Änderung: Configure4Ansible installiert imagemagick und passt Berechtigungen zum Verändern des Lock-Bildes an; TODO: GPO muss angepasst werden (und das CMDLET tut nicht...</t>
+    <t xml:space="preserve">wichtige Änderung: Configure4Ansible installiert imagemagick und passt Berechtigungen zum Verändern des Lock-Bildes an; hat ewig gedauert!</t>
   </si>
   <si>
     <t xml:space="preserve">ISSUES:</t>
@@ -884,8 +891,8 @@
   </sheetPr>
   <dimension ref="A1:G38"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A14" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E34" activeCellId="0" sqref="E34"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1075,7 +1082,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="24" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="46.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
         <v>46</v>
       </c>
@@ -1086,7 +1093,7 @@
         <v>0.4</v>
       </c>
       <c r="D10" s="10" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>47</v>
@@ -1185,7 +1192,7 @@
       </c>
       <c r="D19" s="17" t="n">
         <f aca="false">SUM(D2:D18)</f>
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="E19" s="16"/>
       <c r="F19" s="16"/>
@@ -1258,7 +1265,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="69" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="2" t="s">
         <v>66</v>
       </c>
@@ -1269,7 +1276,7 @@
         <v>0.9</v>
       </c>
       <c r="D28" s="10" t="n">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>67</v>
@@ -1303,7 +1310,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="35.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="2" t="s">
         <v>72</v>
       </c>
@@ -1316,7 +1323,9 @@
       <c r="D31" s="10" t="n">
         <v>9</v>
       </c>
-      <c r="E31" s="14"/>
+      <c r="E31" s="14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
@@ -1325,7 +1334,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="2" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B33" s="10" t="n">
         <v>16</v>
@@ -1334,12 +1343,15 @@
         <v>0.9</v>
       </c>
       <c r="D33" s="10" t="n">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>20</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="2" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B34" s="10" t="n">
         <v>4</v>
@@ -1348,26 +1360,26 @@
         <v>0.9</v>
       </c>
       <c r="D34" s="10" t="n">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="E34" s="14" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="80.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="2" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B37" s="15" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="C37" s="20" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="10" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="C38" s="21" t="n">
         <v>0.9</v>

</xml_diff>